<commit_message>
Mostly done with analysis, need to clean up graphics
</commit_message>
<xml_diff>
--- a/output/ eligible_insts.xlsx
+++ b/output/ eligible_insts.xlsx
@@ -8470,7 +8470,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8627,27 +8627,6 @@
       </c>
       <c r="E7">
         <v>40</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>MT</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>The University of Montana-Western</t>
-        </is>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -10619,7 +10598,7 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10891,7 +10870,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CUNY Medgar Evers College</t>
+          <t>CUNY New York City College of Technology</t>
         </is>
       </c>
       <c r="C13">
@@ -10901,7 +10880,7 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
@@ -11416,7 +11395,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SUNY College of Technology at Delhi</t>
+          <t>SUNY College of Technology at Canton</t>
         </is>
       </c>
       <c r="C38">
@@ -11437,7 +11416,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SUNY Morrisville</t>
+          <t>SUNY College of Technology at Delhi</t>
         </is>
       </c>
       <c r="C39">
@@ -11458,14 +11437,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Tompkins Cortland Community College</t>
+          <t>SUNY Morrisville</t>
         </is>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>40</v>
@@ -11479,7 +11458,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ulster County Community College</t>
+          <t>Tompkins Cortland Community College</t>
         </is>
       </c>
       <c r="C41">
@@ -11500,7 +11479,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SUNY Westchester Community College</t>
+          <t>Ulster County Community College</t>
         </is>
       </c>
       <c r="C42">
@@ -11521,17 +11500,17 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Oswego County BOCES</t>
+          <t>SUNY Westchester Community College</t>
         </is>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E43">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44">
@@ -11542,17 +11521,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Suffolk County Community College</t>
+          <t>Oswego County BOCES</t>
         </is>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E44">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="45">
@@ -11563,17 +11542,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Madison Oneida BOCES-Practical Nursing Program</t>
+          <t>Suffolk County Community College</t>
         </is>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E45">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46">
@@ -11584,7 +11563,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Erie 2 Chautauqua Cattaraugus BOCES-Practical Nursing Program</t>
+          <t>Madison Oneida BOCES-Practical Nursing Program</t>
         </is>
       </c>
       <c r="C46">
@@ -11605,7 +11584,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Schuyler Steuben Chemung Tioga Allegany BOCES</t>
+          <t>Erie 2 Chautauqua Cattaraugus BOCES-Practical Nursing Program</t>
         </is>
       </c>
       <c r="C47">
@@ -11626,7 +11605,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Delaware Chenango Madison Otsego BOCES-Practical Nursing Program</t>
+          <t>Schuyler Steuben Chemung Tioga Allegany BOCES</t>
         </is>
       </c>
       <c r="C48">
@@ -12119,27 +12098,6 @@
         <v>7</v>
       </c>
       <c r="E71">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>NY</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Eastern Suffolk BOCES</t>
-        </is>
-      </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72">
-        <v>7</v>
-      </c>
-      <c r="E72">
         <v>-2</v>
       </c>
     </row>
@@ -13574,7 +13532,7 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -14560,7 +14518,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ohio State University-Lima Campus</t>
+          <t>Ohio State University-Mansfield Campus</t>
         </is>
       </c>
       <c r="C47">
@@ -14581,7 +14539,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Ohio State University-Mansfield Campus</t>
+          <t>Ohio State University-Marion Campus</t>
         </is>
       </c>
       <c r="C48">
@@ -14602,7 +14560,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Ohio State University-Marion Campus</t>
+          <t>Ohio State University-Newark Campus</t>
         </is>
       </c>
       <c r="C49">
@@ -14623,7 +14581,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ohio State University-Newark Campus</t>
+          <t>Ohio University-Eastern Campus</t>
         </is>
       </c>
       <c r="C50">
@@ -14633,7 +14591,7 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51">
@@ -14644,7 +14602,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ohio University-Eastern Campus</t>
+          <t>Ohio University-Chillicothe Campus</t>
         </is>
       </c>
       <c r="C51">
@@ -14665,7 +14623,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Ohio University-Chillicothe Campus</t>
+          <t>Ohio University-Southern Campus</t>
         </is>
       </c>
       <c r="C52">
@@ -14675,7 +14633,7 @@
         <v>1</v>
       </c>
       <c r="E52">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="53">
@@ -14686,7 +14644,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Ohio University-Southern Campus</t>
+          <t>Ohio University-Lancaster Campus</t>
         </is>
       </c>
       <c r="C53">
@@ -14696,7 +14654,7 @@
         <v>1</v>
       </c>
       <c r="E53">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54">
@@ -14707,7 +14665,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Ohio University-Lancaster Campus</t>
+          <t>Ohio University-Zanesville Campus</t>
         </is>
       </c>
       <c r="C54">
@@ -14728,14 +14686,14 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Ohio University-Zanesville Campus</t>
+          <t>Owens Community College</t>
         </is>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E55">
         <v>40</v>
@@ -14749,17 +14707,17 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Owens Community College</t>
+          <t>Cuyahoga Valley Career Center</t>
         </is>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E56">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="57">
@@ -14770,17 +14728,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cuyahoga Valley Career Center</t>
+          <t>Sinclair Community College</t>
         </is>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58">
@@ -14791,14 +14749,14 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Sinclair Community College</t>
+          <t>Stark State College</t>
         </is>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E58">
         <v>40</v>
@@ -14812,7 +14770,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Stark State College</t>
+          <t>Southern State Community College</t>
         </is>
       </c>
       <c r="C59">
@@ -14833,7 +14791,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Southern State Community College</t>
+          <t>Terra State Community College</t>
         </is>
       </c>
       <c r="C60">
@@ -14854,17 +14812,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Terra State Community College</t>
+          <t>Tri-County Adult Career Center</t>
         </is>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E61">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="62">
@@ -14875,7 +14833,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Tri-County Adult Career Center</t>
+          <t>Tri-Rivers Career Center</t>
         </is>
       </c>
       <c r="C62">
@@ -14896,7 +14854,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Tri-Rivers Career Center</t>
+          <t>Upper Valley Career Center</t>
         </is>
       </c>
       <c r="C63">
@@ -14917,17 +14875,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Upper Valley Career Center</t>
+          <t>Washington State Community College</t>
         </is>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="65">
@@ -14938,17 +14896,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Washington State Community College</t>
+          <t>Portage Lakes Career Center</t>
         </is>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E65">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="66">
@@ -14959,7 +14917,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Portage Lakes Career Center</t>
+          <t>Greene County Vocational School District</t>
         </is>
       </c>
       <c r="C66">
@@ -14980,7 +14938,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Greene County Vocational School District</t>
+          <t>Alliance Career Center</t>
         </is>
       </c>
       <c r="C67">
@@ -15001,7 +14959,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Alliance Career Center</t>
+          <t>Knox County Career Center</t>
         </is>
       </c>
       <c r="C68">
@@ -15022,14 +14980,14 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Knox County Career Center</t>
+          <t>Madison Adult Career Center</t>
         </is>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E69">
         <v>-2</v>
@@ -15043,14 +15001,14 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Madison Adult Career Center</t>
+          <t>U S Grant Joint Vocational School</t>
         </is>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E70">
         <v>-2</v>
@@ -15064,7 +15022,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>U S Grant Joint Vocational School</t>
+          <t>Buckeye Joint Vocational School</t>
         </is>
       </c>
       <c r="C71">
@@ -15085,14 +15043,14 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Buckeye Joint Vocational School</t>
+          <t>Sandusky Career Center</t>
         </is>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E72">
         <v>-2</v>
@@ -15106,14 +15064,14 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Sandusky Career Center</t>
+          <t>Mid-EastCTC-Adult Education</t>
         </is>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E73">
         <v>-2</v>
@@ -15127,7 +15085,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Mid-EastCTC-Adult Education</t>
+          <t>Polaris Career Center</t>
         </is>
       </c>
       <c r="C74">
@@ -15148,7 +15106,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Polaris Career Center</t>
+          <t>Eastland-Fairfield Career and Technical Schools</t>
         </is>
       </c>
       <c r="C75">
@@ -15169,7 +15127,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Eastland-Fairfield Career and Technical Schools</t>
+          <t>Mahoning County Career and Technical Center</t>
         </is>
       </c>
       <c r="C76">
@@ -15190,7 +15148,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Mahoning County Career and Technical Center</t>
+          <t>Pickaway Ross Joint Vocational School District</t>
         </is>
       </c>
       <c r="C77">
@@ -15211,7 +15169,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Pickaway Ross Joint Vocational School District</t>
+          <t>Pioneer Career and Technology Center</t>
         </is>
       </c>
       <c r="C78">
@@ -15232,7 +15190,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Pioneer Career and Technology Center</t>
+          <t>Scioto County Career Technical Center</t>
         </is>
       </c>
       <c r="C79">
@@ -15253,7 +15211,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Scioto County Career Technical Center</t>
+          <t>Trumbull Career &amp; Technical Center</t>
         </is>
       </c>
       <c r="C80">
@@ -15274,14 +15232,14 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Trumbull Career &amp; Technical Center</t>
+          <t>Warren County Career Center</t>
         </is>
       </c>
       <c r="C81">
         <v>1</v>
       </c>
       <c r="D81">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E81">
         <v>-2</v>
@@ -15295,14 +15253,14 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Warren County Career Center</t>
+          <t>Pike County Joint Vocational School District</t>
         </is>
       </c>
       <c r="C82">
         <v>1</v>
       </c>
       <c r="D82">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E82">
         <v>-2</v>
@@ -15316,7 +15274,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Pike County Joint Vocational School District</t>
+          <t>Lorain County Joint Vocational School District</t>
         </is>
       </c>
       <c r="C83">
@@ -15337,7 +15295,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Lorain County Joint Vocational School District</t>
+          <t>Penta County Joint Vocational School</t>
         </is>
       </c>
       <c r="C84">
@@ -15358,7 +15316,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Penta County Joint Vocational School</t>
+          <t>Career and Technology Education Centers of Licking County</t>
         </is>
       </c>
       <c r="C85">
@@ -15379,7 +15337,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Career and Technology Education Centers of Licking County</t>
+          <t>Northern Career Institute</t>
         </is>
       </c>
       <c r="C86">
@@ -15400,7 +15358,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Northern Career Institute</t>
+          <t>Washington County Career Center-Adult Technical Training</t>
         </is>
       </c>
       <c r="C87">
@@ -15421,7 +15379,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Washington County Career Center-Adult Technical Training</t>
+          <t>Ohio Technical Center at Vantage Career Center</t>
         </is>
       </c>
       <c r="C88">
@@ -15442,7 +15400,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Ohio Technical Center at Vantage Career Center</t>
+          <t>Vanguard-Sentinel Adult Career and Technology Center</t>
         </is>
       </c>
       <c r="C89">
@@ -15463,7 +15421,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Vanguard-Sentinel Adult Career and Technology Center</t>
+          <t>Wayne County Schools Career Center</t>
         </is>
       </c>
       <c r="C90">
@@ -15484,7 +15442,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Wayne County Schools Career Center</t>
+          <t>Four County Career Center</t>
         </is>
       </c>
       <c r="C91">
@@ -15494,27 +15452,6 @@
         <v>7</v>
       </c>
       <c r="E91">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>OH</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Four County Career Center</t>
-        </is>
-      </c>
-      <c r="C92">
-        <v>1</v>
-      </c>
-      <c r="D92">
-        <v>7</v>
-      </c>
-      <c r="E92">
         <v>-2</v>
       </c>
     </row>
@@ -17830,7 +17767,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Forbes Road Career and Technology Center</t>
+          <t>Hazleton Area Career Center</t>
         </is>
       </c>
       <c r="C44">
@@ -17851,7 +17788,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Crawford County Career and Technical Center Practical Nursing Program</t>
+          <t>Forbes Road Career and Technology Center</t>
         </is>
       </c>
       <c r="C45">
@@ -23206,7 +23143,7 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -23289,17 +23226,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>James Rumsey Technical Institute</t>
+          <t>Glenville State College</t>
         </is>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>-2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
@@ -23310,7 +23247,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ralph R Willis Career and Technical Center</t>
+          <t>James Rumsey Technical Institute</t>
         </is>
       </c>
       <c r="C5">
@@ -23331,14 +23268,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mercer County Technical Education Center</t>
+          <t>Ralph R Willis Career and Technical Center</t>
         </is>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>-2</v>
@@ -23352,14 +23289,14 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Monongalia County Technical Education Center</t>
+          <t>Mercer County Technical Education Center</t>
         </is>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>-2</v>
@@ -23373,17 +23310,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>West Virginia University at Parkersburg</t>
+          <t>Monongalia County Technical Education Center</t>
         </is>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E8">
-        <v>33</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9">
@@ -23394,7 +23331,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Potomac State College of West Virginia University</t>
+          <t>West Virginia University at Parkersburg</t>
         </is>
       </c>
       <c r="C9">
@@ -23404,7 +23341,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
@@ -23415,17 +23352,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Academy of Careers and Technology</t>
+          <t>Potomac State College of West Virginia University</t>
         </is>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -23436,17 +23373,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Southern West Virginia Community and Technical College</t>
+          <t>Academy of Careers and Technology</t>
         </is>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E11">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="12">
@@ -23457,7 +23394,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Fred W Eberle Technical Center</t>
+          <t>Southern West Virginia Community and Technical College</t>
         </is>
       </c>
       <c r="C12">
@@ -23467,7 +23404,7 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -23478,7 +23415,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>West Virginia Northern Community College</t>
+          <t>Fred W Eberle Technical Center</t>
         </is>
       </c>
       <c r="C13">
@@ -23488,7 +23425,7 @@
         <v>4</v>
       </c>
       <c r="E13">
-        <v>40</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14">
@@ -23499,17 +23436,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Wood County School of Practical Nursing</t>
+          <t>West Virginia Northern Community College</t>
         </is>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>-2</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15">
@@ -23520,14 +23457,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Roane-Jackson Technical Center</t>
+          <t>Wood County School of Practical Nursing</t>
         </is>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>-2</v>
@@ -23541,14 +23478,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mineral County Vocational Technical Center</t>
+          <t>Roane-Jackson Technical Center</t>
         </is>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>-2</v>
@@ -23562,7 +23499,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Fayette Institute of Technology</t>
+          <t>Mineral County Vocational Technical Center</t>
         </is>
       </c>
       <c r="C17">
@@ -23583,7 +23520,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>United Technical Center</t>
+          <t>Fayette Institute of Technology</t>
         </is>
       </c>
       <c r="C18">
@@ -23604,7 +23541,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Putnam Career and Technical Center</t>
+          <t>United Technical Center</t>
         </is>
       </c>
       <c r="C19">
@@ -23625,14 +23562,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Carver Career Center</t>
+          <t>Putnam Career and Technical Center</t>
         </is>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>-2</v>
@@ -23646,14 +23583,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Garnet Career Center</t>
+          <t>Carver Career Center</t>
         </is>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <v>-2</v>
@@ -23667,14 +23604,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Eastern West Virginia Community and Technical College</t>
+          <t>Garnet Career Center</t>
         </is>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>-2</v>
@@ -23688,7 +23625,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Pierpont Community and Technical College</t>
+          <t>Eastern West Virginia Community and Technical College</t>
         </is>
       </c>
       <c r="C23">
@@ -23709,7 +23646,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mountwest Community and Technical College</t>
+          <t>Pierpont Community and Technical College</t>
         </is>
       </c>
       <c r="C24">
@@ -23730,14 +23667,14 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>John D Rockefeller IV Career Center</t>
+          <t>Mountwest Community and Technical College</t>
         </is>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>-2</v>
@@ -23751,14 +23688,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Blue Ridge Community and Technical College</t>
+          <t>John D Rockefeller IV Career Center</t>
         </is>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E26">
         <v>-2</v>
@@ -23772,7 +23709,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>New River Community and Technical College</t>
+          <t>Blue Ridge Community and Technical College</t>
         </is>
       </c>
       <c r="C27">
@@ -23793,7 +23730,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BridgeValley Community &amp; Technical College</t>
+          <t>New River Community and Technical College</t>
         </is>
       </c>
       <c r="C28">
@@ -23814,14 +23751,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Mingo Extended Learning Center</t>
+          <t>BridgeValley Community &amp; Technical College</t>
         </is>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <v>-2</v>
@@ -23835,7 +23772,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Randolph Technical Center</t>
+          <t>Mingo Extended Learning Center</t>
         </is>
       </c>
       <c r="C30">
@@ -23845,6 +23782,27 @@
         <v>7</v>
       </c>
       <c r="E30">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>WV</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Randolph Technical Center</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
         <v>-2</v>
       </c>
     </row>
@@ -23855,7 +23813,7 @@
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -24222,6 +24180,27 @@
       </c>
       <c r="E17">
         <v>40</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WI</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>University of Wisconsin-Parkside Flex</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>
@@ -26876,7 +26855,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Ukiah Adult School</t>
+          <t>Riverside County Office of Education-School of Career Education</t>
         </is>
       </c>
       <c r="C126">
@@ -26897,14 +26876,14 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Riverside County Office of Education-School of Career Education</t>
+          <t>Tri-Community Adult Education</t>
         </is>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
       <c r="D127">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E127">
         <v>-2</v>
@@ -26918,14 +26897,14 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Tri-Community Adult Education</t>
+          <t>Butte County Regional Occupational Program</t>
         </is>
       </c>
       <c r="C128">
         <v>1</v>
       </c>
       <c r="D128">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E128">
         <v>-2</v>
@@ -26939,14 +26918,14 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Butte County Regional Occupational Program</t>
+          <t>Clovis Community College</t>
         </is>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
       <c r="D129">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E129">
         <v>-2</v>
@@ -26960,14 +26939,14 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Clovis Community College</t>
+          <t>Baldy View Regional Occupational Program</t>
         </is>
       </c>
       <c r="C130">
         <v>1</v>
       </c>
       <c r="D130">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E130">
         <v>-2</v>
@@ -28106,7 +28085,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -29617,7 +29596,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>D A Dorsey Technical College</t>
+          <t>Aparicio-Levy Technical College</t>
         </is>
       </c>
       <c r="C72">
@@ -29638,7 +29617,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Aparicio-Levy Technical College</t>
+          <t>Treasure Coast Technical College</t>
         </is>
       </c>
       <c r="C73">
@@ -29659,7 +29638,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Treasure Coast Technical College</t>
+          <t>South Dade Technical College</t>
         </is>
       </c>
       <c r="C74">
@@ -29680,14 +29659,14 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>South Dade Technical College</t>
+          <t>Gadsden Technical Institute</t>
         </is>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E75">
         <v>-2</v>
@@ -29701,37 +29680,16 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Gadsden Technical Institute</t>
+          <t>Suncoast Technical Education Center</t>
         </is>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E76">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>FL</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Suncoast Technical Education Center</t>
-        </is>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77">
-        <v>7</v>
-      </c>
-      <c r="E77">
         <v>-2</v>
       </c>
     </row>

</xml_diff>